<commit_message>
add new A321neo flight model and EFB update
</commit_message>
<xml_diff>
--- a/tools/MOI_Airbus_A32X_family.xlsx
+++ b/tools/MOI_Airbus_A32X_family.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\LVFR-flybywire\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D21F87CF-5673-478F-A463-2E602DA6BE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF245286-F766-4499-AEE1-5F8609B63167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24885" yWindow="-4710" windowWidth="21600" windowHeight="11295" xr2:uid="{6B2DA0DD-10D3-4D1C-9A69-9F16A5979071}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6B2DA0DD-10D3-4D1C-9A69-9F16A5979071}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -428,7 +428,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,15 +627,15 @@
       </c>
       <c r="D20">
         <f>((K1*B20)^2 /4)*B23/32.2</f>
-        <v>989090.40128281387</v>
+        <v>1210170.2680241819</v>
       </c>
       <c r="E20">
         <f>((K2*B21)^2 /4)*B23/32.2</f>
-        <v>3439991.3350072354</v>
+        <v>4208892.5648124218</v>
       </c>
       <c r="F20">
         <f>((K3*B22)^2 /4)*B23/32.2</f>
-        <v>3763090.9120604489</v>
+        <v>4604210.83021452</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <v>93697</v>
+        <v>114640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add efb for LR variant
</commit_message>
<xml_diff>
--- a/tools/MOI_Airbus_A32X_family.xlsx
+++ b/tools/MOI_Airbus_A32X_family.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\LVFR-flybywire\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF245286-F766-4499-AEE1-5F8609B63167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F4316A-0EF1-455B-B110-BD87BEC7C3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6B2DA0DD-10D3-4D1C-9A69-9F16A5979071}"/>
+    <workbookView xWindow="-38520" yWindow="-5475" windowWidth="38640" windowHeight="21120" xr2:uid="{6B2DA0DD-10D3-4D1C-9A69-9F16A5979071}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -627,15 +627,15 @@
       </c>
       <c r="D20">
         <f>((K1*B20)^2 /4)*B23/32.2</f>
-        <v>1210170.2680241819</v>
+        <v>1166467.3291754371</v>
       </c>
       <c r="E20">
         <f>((K2*B21)^2 /4)*B23/32.2</f>
-        <v>4208892.5648124218</v>
+        <v>4056896.6190838502</v>
       </c>
       <c r="F20">
         <f>((K3*B22)^2 /4)*B23/32.2</f>
-        <v>4604210.83021452</v>
+        <v>4437938.7363808835</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <v>114640</v>
+        <v>110500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>